<commit_message>
updated powershell vs shell
</commit_message>
<xml_diff>
--- a/Powershell/Powershell vs Shell.xlsx
+++ b/Powershell/Powershell vs Shell.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cowsik.shanmugam\Documents\Learning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cowsik.shanmugam\Documents\GitHub\documentation\Powershell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{741EE4D1-9545-4070-922E-2FC3D8DCB37D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DE9B183-9886-469B-BCC3-26ED69798E0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="747" xr2:uid="{96148EC0-1EC1-4FC1-9B42-FC0352C7E8CA}"/>
   </bookViews>
@@ -1575,7 +1575,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1601,7 +1601,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1942,7 +1941,7 @@
   <dimension ref="A1:E65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3180,12 +3179,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.81640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.54296875" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.81640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43.36328125" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.26953125" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="9"/>
+    <col min="1" max="1" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3300,14 +3298,14 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="21.81640625" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.08984375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.6328125" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="45.08984375" style="5" customWidth="1"/>
     <col min="5" max="5" width="35.1796875" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="8.7265625" style="5"/>
@@ -3330,7 +3328,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" ht="26.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="6" t="s">
         <v>393</v>
       </c>
@@ -3364,7 +3362,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="6" t="s">
         <v>467</v>
       </c>
@@ -3464,12 +3462,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.81640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.26953125" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.6328125" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.36328125" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="9"/>
+    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3720,20 +3717,19 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.81640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.6328125" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.6328125" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.54296875" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.453125" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.81640625" style="9"/>
+    <col min="1" max="1" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4582,12 +4578,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.81640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.54296875" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.1796875" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.26953125" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.36328125" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.81640625" style="9"/>
+    <col min="1" max="1" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4826,7 +4821,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>